<commit_message>
add initial weights strategy
</commit_message>
<xml_diff>
--- a/操作记录.xlsx
+++ b/操作记录.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>模型</t>
     <rPh sb="0" eb="1">
@@ -99,6 +99,10 @@
   </si>
   <si>
     <t>0.179859+新的初始化</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>train-logloss</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -155,7 +159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -188,6 +192,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -467,152 +474,169 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F74"/>
+  <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="136" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="136" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" style="1" customWidth="1"/>
     <col min="2" max="2" width="52.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="23.33203125" style="9" customWidth="1"/>
+    <col min="4" max="4" width="16.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="80" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:7" ht="80" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
         <v>0.20552973456596699</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>0.19209200000000001</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="1">
         <v>8000</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="9"/>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="12"/>
       <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2">
+      <c r="D3" s="2">
         <v>0.20525302019858299</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="2">
         <v>0.192075</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F3" s="1">
         <v>6800</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="9"/>
+    <row r="4" spans="1:7" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="12"/>
       <c r="B4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="2">
+      <c r="D4" s="2">
         <v>0.20432016110008999</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E4" s="2">
         <v>0.19167699999999999</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="2">
         <v>7296</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="216" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9"/>
+    <row r="5" spans="1:7" ht="216" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="12"/>
       <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="6">
+      <c r="D5" s="6">
         <v>0.19274793383</v>
       </c>
-      <c r="D5" s="11">
+      <c r="E5" s="11">
         <v>0.17985899999999999</v>
       </c>
-      <c r="E5" s="2">
+      <c r="F5" s="2">
         <v>5400</v>
       </c>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="9"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="12"/>
       <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="7">
+      <c r="D6" s="7">
         <v>0.19533626471320301</v>
       </c>
-      <c r="D6" s="7">
+      <c r="E6" s="7">
         <v>0.182666</v>
       </c>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="9"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="12"/>
       <c r="B7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="1">
+      <c r="D7" s="1">
         <v>0.19964279800000001</v>
       </c>
-      <c r="D7" s="8">
+      <c r="E7" s="8">
         <v>0.185694</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="12"/>
       <c r="B8" s="4"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C8" s="9">
+        <v>0.139407584576</v>
+      </c>
+      <c r="D8" s="9">
+        <v>0.19472321703199999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="12"/>
       <c r="B9" s="4"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="12"/>
       <c r="B10" s="4"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="12"/>
       <c r="B11" s="4"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="12"/>
       <c r="B12" s="4"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="12"/>
       <c r="B13" s="4"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="12"/>
       <c r="B14" s="4"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B15" s="4"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B16" s="4"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.2">
@@ -791,7 +815,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A2:A14"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>